<commit_message>
Fin rapport E2 Fin rapport E1
</commit_message>
<xml_diff>
--- a/gestion_projet/planning_previsionnel2.xlsx
+++ b/gestion_projet/planning_previsionnel2.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665"/>
+    <workbookView xWindow="480" yWindow="345" windowWidth="19815" windowHeight="7665" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="V1" sheetId="1" r:id="rId1"/>
+    <sheet name="V2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>Tâches</t>
   </si>
@@ -106,13 +105,19 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Livrables</t>
+  </si>
+  <si>
+    <t>S. 19/12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,8 +133,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,6 +160,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -341,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -388,38 +406,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:Q14"/>
     </sheetView>
   </sheetViews>
@@ -785,7 +818,7 @@
       </c>
     </row>
     <row r="3" spans="2:17" ht="30">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="23" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -804,10 +837,10 @@
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
-      <c r="Q3" s="17"/>
+      <c r="Q3" s="16"/>
     </row>
     <row r="4" spans="2:17" ht="30" customHeight="1">
-      <c r="B4" s="18"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
@@ -824,10 +857,10 @@
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
-      <c r="Q4" s="17"/>
+      <c r="Q4" s="16"/>
     </row>
     <row r="5" spans="2:17" ht="30" customHeight="1">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -846,10 +879,10 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
-      <c r="Q5" s="17"/>
+      <c r="Q5" s="16"/>
     </row>
     <row r="6" spans="2:17" ht="33" customHeight="1">
-      <c r="B6" s="19"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
@@ -866,10 +899,10 @@
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
-      <c r="Q6" s="17"/>
+      <c r="Q6" s="16"/>
     </row>
     <row r="7" spans="2:17" ht="36" customHeight="1">
-      <c r="B7" s="19"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
@@ -886,10 +919,10 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
-      <c r="Q7" s="17"/>
+      <c r="Q7" s="16"/>
     </row>
     <row r="8" spans="2:17" ht="30" customHeight="1">
-      <c r="B8" s="19"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
@@ -906,10 +939,10 @@
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
-      <c r="Q8" s="17"/>
+      <c r="Q8" s="16"/>
     </row>
     <row r="9" spans="2:17" ht="30" customHeight="1">
-      <c r="B9" s="19"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
@@ -926,10 +959,10 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
-      <c r="Q9" s="17"/>
+      <c r="Q9" s="16"/>
     </row>
     <row r="10" spans="2:17" ht="30.75" customHeight="1">
-      <c r="B10" s="19"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
@@ -946,10 +979,10 @@
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
-      <c r="Q10" s="17"/>
+      <c r="Q10" s="16"/>
     </row>
     <row r="11" spans="2:17" ht="30">
-      <c r="B11" s="19"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
@@ -966,10 +999,10 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
-      <c r="Q11" s="17"/>
+      <c r="Q11" s="16"/>
     </row>
     <row r="12" spans="2:17" ht="30.75" customHeight="1">
-      <c r="B12" s="18"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
@@ -986,10 +1019,10 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
-      <c r="Q12" s="17"/>
+      <c r="Q12" s="16"/>
     </row>
     <row r="13" spans="2:17" ht="30.75" customHeight="1">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1008,27 +1041,27 @@
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
-      <c r="Q13" s="20"/>
+      <c r="Q13" s="17"/>
     </row>
     <row r="14" spans="2:17" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B14" s="21"/>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="26"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1043,24 +1076,396 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="1.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="27.5703125" style="10" customWidth="1"/>
+    <col min="4" max="7" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="1.42578125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="5.25" customHeight="1" thickBot="1">
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+    </row>
+    <row r="2" spans="1:18" s="3" customFormat="1">
+      <c r="A2" s="31"/>
+      <c r="B2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="31"/>
+    </row>
+    <row r="3" spans="1:18" ht="30">
+      <c r="A3" s="29"/>
+      <c r="B3" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="29"/>
+    </row>
+    <row r="4" spans="1:18" ht="30" customHeight="1">
+      <c r="A4" s="29"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="29"/>
+    </row>
+    <row r="5" spans="1:18" ht="30" customHeight="1">
+      <c r="A5" s="29"/>
+      <c r="B5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="29"/>
+    </row>
+    <row r="6" spans="1:18" ht="30" customHeight="1">
+      <c r="A6" s="29"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="29"/>
+    </row>
+    <row r="7" spans="1:18" ht="33" customHeight="1">
+      <c r="A7" s="29"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="29"/>
+    </row>
+    <row r="8" spans="1:18" ht="36" customHeight="1">
+      <c r="A8" s="29"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="29"/>
+    </row>
+    <row r="9" spans="1:18" ht="30" customHeight="1">
+      <c r="A9" s="29"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="29"/>
+    </row>
+    <row r="10" spans="1:18" ht="30" customHeight="1">
+      <c r="A10" s="29"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="29"/>
+    </row>
+    <row r="11" spans="1:18" ht="30.75" customHeight="1">
+      <c r="A11" s="29"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="29"/>
+    </row>
+    <row r="12" spans="1:18" ht="30">
+      <c r="A12" s="29"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="29"/>
+    </row>
+    <row r="13" spans="1:18" ht="30.75" customHeight="1">
+      <c r="A13" s="29"/>
+      <c r="B13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="29"/>
+    </row>
+    <row r="14" spans="1:18" ht="29.25" customHeight="1" thickBot="1">
+      <c r="A14" s="29"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="29"/>
+    </row>
+    <row r="15" spans="1:18" ht="3.75" customHeight="1">
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B5:B12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>